<commit_message>
only show totalProtocol left
</commit_message>
<xml_diff>
--- a/app/src/main/assets/protocol_total.xlsx
+++ b/app/src/main/assets/protocol_total.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinov\OneDrive\Рабочий стол\alex big dick\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinov\AndroidStudioProjects\ATour\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Федерация спортивного туризма России</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Сложность/Новизна/Безопасность/Напряженность/Полезность</t>
   </si>
   <si>
-    <t>Маршрут - водный (1-6 категория), 0840021811Я</t>
-  </si>
-  <si>
     <t>Результат</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
   </si>
   <si>
     <t>Место 3-4 кс</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Чемпионат Уральского и Приволжского ФО (зональные соревнования) 2020 г.     </t>
   </si>
   <si>
     <t>Безопасность</t>
@@ -471,6 +465,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -492,80 +555,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -937,7 +931,7 @@
   <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="Q4" sqref="Q4:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,14 +950,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="53" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
       <c r="I1" s="27"/>
@@ -977,12 +971,12 @@
       <c r="Q1" s="27"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
@@ -996,12 +990,12 @@
       <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
@@ -1015,44 +1009,40 @@
       <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="29"/>
-      <c r="H4" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
+      <c r="H4" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
       <c r="N4" s="29"/>
       <c r="O4" s="29"/>
       <c r="P4" s="29"/>
-      <c r="Q4" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" s="49"/>
+      <c r="Q4" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="53"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
@@ -1066,41 +1056,41 @@
       <c r="Q5" s="27"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
-      <c r="L6" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
+      <c r="L6" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
       <c r="P6" s="35"/>
       <c r="Q6" s="30"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="58" t="s">
+      <c r="B7" s="47"/>
+      <c r="C7" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
@@ -1114,14 +1104,14 @@
       <c r="Q7" s="30"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
@@ -1135,104 +1125,104 @@
       <c r="Q8" s="31"/>
     </row>
     <row r="9" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="P9" s="43" t="s">
+      <c r="R9" s="64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="55" t="s">
+      <c r="J10" s="42"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="N10" s="42"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
     </row>
     <row r="11" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="37" t="s">
         <v>6</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K11" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
+        <v>34</v>
+      </c>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
     </row>
     <row r="12" spans="1:22" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -1651,7 +1641,7 @@
         <v>#REF!</v>
       </c>
       <c r="N26" s="20" t="e">
-        <f t="shared" ref="N14:N36" si="0">G26+H26+I26+J26+K26+L26+M26</f>
+        <f t="shared" ref="N26:N36" si="0">G26+H26+I26+J26+K26+L26+M26</f>
         <v>#REF!</v>
       </c>
       <c r="O26" s="21"/>
@@ -2364,9 +2354,9 @@
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="36"/>
       <c r="J42" s="36"/>
     </row>
@@ -2375,63 +2365,63 @@
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
       <c r="F43" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="36"/>
       <c r="J43" s="36"/>
-      <c r="K43" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
+      <c r="K43" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="L43" s="70"/>
+      <c r="M43" s="70"/>
+      <c r="N43" s="70"/>
+      <c r="O43" s="70"/>
+      <c r="P43" s="70"/>
+      <c r="Q43" s="70"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
       <c r="F44" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
-      <c r="Q44" s="39"/>
+      <c r="K44" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="F45" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="L45" s="40"/>
-      <c r="M45" s="40"/>
-      <c r="N45" s="40"/>
-      <c r="O45" s="40"/>
-      <c r="P45" s="40"/>
-      <c r="Q45" s="40"/>
+      <c r="K45" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="L45" s="63"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="63"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="63"/>
+      <c r="Q45" s="63"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
@@ -2670,19 +2660,14 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="37">
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="K44:Q44"/>
+    <mergeCell ref="K45:Q45"/>
+    <mergeCell ref="R9:R11"/>
+    <mergeCell ref="Q9:Q11"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="O9:O11"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="K43:Q43"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="F42:H42"/>
@@ -2699,14 +2684,19 @@
     <mergeCell ref="H4:M4"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K44:Q44"/>
-    <mergeCell ref="K45:Q45"/>
-    <mergeCell ref="R9:R11"/>
-    <mergeCell ref="Q9:Q11"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="O9:O11"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="K43:Q43"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.31496062992125984" bottom="0.31496062992125984" header="0" footer="0"/>

</xml_diff>